<commit_message>
updated to async fetch method!
</commit_message>
<xml_diff>
--- a/data-structur.xlsx
+++ b/data-structur.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\Projects\WebDev\2021\210206_BirDict\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464D0B39-F998-4FEA-897C-461D24BB9CDA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E7143C-8656-49EE-B177-4B7D98E07980}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{784D83DC-DBDD-470F-9266-ADF61A2E4B6A}"/>
+    <workbookView xWindow="12105" yWindow="690" windowWidth="35985" windowHeight="17910" xr2:uid="{784D83DC-DBDD-470F-9266-ADF61A2E4B6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Munka1!$B$5:$L$76</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Munka1!$B$5:$M$76</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="171">
   <si>
     <t>ID</t>
   </si>
@@ -514,6 +514,33 @@
   </si>
   <si>
     <t>test-4</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>peterfulop</t>
+  </si>
+  <si>
+    <t>mrpeterfulop@gmail.com</t>
+  </si>
+  <si>
+    <t>8f0593d009b9ba416d39a25cac472264</t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> adca5734c8ec4916fd133abb91dce99b</t>
+  </si>
+  <si>
+    <t>adca5734c8ec4916fd133abb91dce99b</t>
   </si>
 </sst>
 </file>
@@ -523,7 +550,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -541,8 +568,17 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -564,6 +600,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -685,10 +727,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -761,8 +804,20 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hivatkozás" xfId="1" builtinId="8"/>
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1075,1976 +1130,2266 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB3B0B2-54B0-4330-B127-9A7406DC2F48}">
-  <dimension ref="B5:AA80"/>
+  <dimension ref="B5:AB80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.140625" customWidth="1"/>
-    <col min="14" max="14" width="4" customWidth="1"/>
-    <col min="15" max="15" width="4.42578125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="20.42578125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.42578125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="5.85546875" customWidth="1"/>
-    <col min="26" max="26" width="18.42578125" customWidth="1"/>
-    <col min="27" max="27" width="9.5703125" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.140625" customWidth="1"/>
+    <col min="15" max="15" width="4" customWidth="1"/>
+    <col min="16" max="16" width="35.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.42578125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="30" style="1" customWidth="1"/>
+    <col min="19" max="19" width="33.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="26.140625" customWidth="1"/>
+    <col min="22" max="22" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.85546875" customWidth="1"/>
+    <col min="27" max="27" width="18.42578125" customWidth="1"/>
+    <col min="28" max="28" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="E5" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="F5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="G5" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="H5" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="I5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="J5" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="K5" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="L5" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="M5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="O5" s="19" t="s">
+      <c r="P5" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="P5" s="19" t="s">
+      <c r="Q5" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="Q5" s="20" t="s">
+      <c r="R5" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="R5" s="20" t="s">
+      <c r="S5" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="S5" s="19" t="s">
+      <c r="T5" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="U5" s="16" t="s">
+      <c r="V5" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="V5" s="16" t="s">
+      <c r="W5" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="W5" s="16" t="s">
+      <c r="X5" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="Y5" s="14" t="s">
+      <c r="Z5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="Z5" s="16" t="s">
+      <c r="AA5" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="AA5" s="14" t="s">
+      <c r="AB5" s="14" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="2"/>
+      <c r="F6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="2"/>
+      <c r="I6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" s="3">
+        <v>21</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="3">
         <v>44231.506944444445</v>
       </c>
-      <c r="O6" s="21">
+      <c r="P6" s="21">
         <v>1</v>
       </c>
-      <c r="P6" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q6" s="23" t="s">
-        <v>21</v>
+      <c r="Q6" s="22" t="s">
+        <v>5</v>
       </c>
       <c r="R6" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="S6" s="24">
+        <v>21</v>
+      </c>
+      <c r="S6" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="T6" s="24">
         <v>43834.604166666664</v>
       </c>
-      <c r="U6" s="4">
+      <c r="V6" s="4">
         <v>1</v>
       </c>
-      <c r="V6" s="5" t="s">
+      <c r="W6" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="W6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y6" s="4">
+      <c r="X6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z6" s="4">
         <v>1</v>
       </c>
-      <c r="Z6" s="5" t="s">
+      <c r="AA6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="AA6" s="6" t="s">
+      <c r="AB6" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>2</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="2"/>
+      <c r="I7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L7" s="3">
+        <v>21</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M7" s="3">
         <v>44232.506944444445</v>
       </c>
-      <c r="O7" s="4">
+      <c r="P7" s="4">
         <v>2</v>
       </c>
-      <c r="P7" s="10" t="s">
+      <c r="Q7" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="Q7" s="5" t="s">
+      <c r="R7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="R7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="S7" s="11">
+      <c r="S7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="T7" s="11">
         <v>43835.489583333336</v>
       </c>
-      <c r="U7" s="4">
+      <c r="V7" s="4">
         <v>2</v>
       </c>
-      <c r="V7" s="5" t="s">
+      <c r="W7" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="W7" s="6" t="s">
+      <c r="X7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Y7" s="4">
+      <c r="Z7" s="4">
         <v>2</v>
       </c>
-      <c r="Z7" s="5" t="s">
+      <c r="AA7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="AA7" s="6" t="s">
+      <c r="AB7" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>3</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D8" s="1">
         <v>1</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="2"/>
+      <c r="I8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L8" s="3">
+        <v>21</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="3">
         <v>44233.506944444445</v>
       </c>
-      <c r="O8" s="4">
+      <c r="P8" s="4">
         <v>3</v>
       </c>
-      <c r="P8" s="10" t="s">
+      <c r="Q8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="Q8" s="5" t="s">
+      <c r="R8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="R8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="S8" s="11">
+      <c r="S8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="T8" s="11">
         <v>43836.836111111108</v>
       </c>
-      <c r="U8" s="4">
+      <c r="V8" s="4">
         <v>3</v>
       </c>
-      <c r="V8" s="5" t="s">
+      <c r="W8" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="W8" s="6" t="s">
+      <c r="X8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Y8" s="4">
+      <c r="Z8" s="4">
         <v>3</v>
       </c>
-      <c r="Z8" s="5" t="s">
+      <c r="AA8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="AA8" s="6" t="s">
+      <c r="AB8" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>4</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D9" s="1">
         <v>1</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="2"/>
+      <c r="I9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L9" s="3">
+        <v>21</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" s="3">
         <v>44234.506944444445</v>
       </c>
-      <c r="O9" s="4">
+      <c r="P9" s="4">
         <v>4</v>
       </c>
-      <c r="P9" s="10" t="s">
+      <c r="Q9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="Q9" s="5" t="s">
+      <c r="R9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="R9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="S9" s="11">
+      <c r="S9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="T9" s="11">
         <v>43831.488888888889</v>
       </c>
-      <c r="U9" s="4">
+      <c r="V9" s="4">
         <v>4</v>
       </c>
-      <c r="V9" s="5" t="s">
+      <c r="W9" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="W9" s="6" t="s">
+      <c r="X9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="Y9" s="4">
+      <c r="Z9" s="4">
         <v>4</v>
       </c>
-      <c r="Z9" s="5" t="s">
+      <c r="AA9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AA9" s="6" t="s">
+      <c r="AB9" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>5</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D10" s="1">
         <v>4</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="2"/>
+      <c r="I10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L10" s="3">
+      <c r="L10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" s="3">
         <v>44235.506944444445</v>
       </c>
-      <c r="O10" s="7">
-        <v>5</v>
-      </c>
-      <c r="P10" s="8" t="s">
+      <c r="P10" s="7">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="Q10" s="8" t="s">
-        <v>21</v>
-      </c>
       <c r="R10" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="S10" s="25">
-        <v>44263.840277777781</v>
-      </c>
-      <c r="U10" s="7">
-        <v>5</v>
-      </c>
-      <c r="V10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="S10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="T10" s="25">
+        <v>44263.840277777781</v>
+      </c>
+      <c r="V10" s="7">
+        <v>5</v>
+      </c>
+      <c r="W10" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="W10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y10" s="4">
-        <v>5</v>
-      </c>
-      <c r="Z10" s="5" t="s">
+      <c r="X10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z10" s="4">
+        <v>5</v>
+      </c>
+      <c r="AA10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AA10" s="6" t="s">
+      <c r="AB10" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>6</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D11" s="1">
         <v>4</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="2"/>
+      <c r="F11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="2"/>
+      <c r="I11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L11" s="3">
+      <c r="L11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M11" s="3">
         <v>44236.506944444445</v>
       </c>
-      <c r="Y11" s="7">
+      <c r="Z11" s="7">
         <v>6</v>
       </c>
-      <c r="Z11" s="8" t="s">
+      <c r="AA11" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="AA11" s="9" t="s">
+      <c r="AB11" s="9" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>7</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D12" s="1">
         <v>4</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="2"/>
+      <c r="I12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L12" s="3">
+      <c r="L12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12" s="3">
         <v>44237.506944444445</v>
       </c>
     </row>
-    <row r="13" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>8</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D13" s="1">
         <v>4</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="2"/>
+      <c r="F13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="2"/>
+      <c r="I13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L13" s="3">
+      <c r="L13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13" s="3">
         <v>44238.506944444445</v>
       </c>
     </row>
-    <row r="14" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>9</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D14" s="1">
         <v>4</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="2"/>
+      <c r="F14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="2"/>
+      <c r="I14" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" s="3">
+      <c r="L14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M14" s="3">
         <v>44239.506944444445</v>
       </c>
-    </row>
-    <row r="15" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="P14" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="R14" s="26" t="s">
+        <v>163</v>
+      </c>
+      <c r="S14" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="T14" s="26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>10</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D15" s="1">
         <v>4</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="2"/>
+      <c r="F15" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="2"/>
+      <c r="I15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L15" s="3">
+      <c r="L15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M15" s="3">
         <v>44240.506944444445</v>
       </c>
-    </row>
-    <row r="16" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="P15" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q15" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="R15" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="S15" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="T15" s="24">
+        <v>44197.76803240741</v>
+      </c>
+    </row>
+    <row r="16" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>11</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D16" s="5">
         <v>2</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L16" s="3">
+      <c r="L16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M16" s="3">
         <v>44241.506944444445</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P16" s="4"/>
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="28"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>12</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D17" s="5">
         <v>2</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="I17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L17" s="3">
+      <c r="L17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M17" s="3">
         <v>44242.506944444445</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P17" s="4"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="28"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>13</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D18" s="5">
         <v>2</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="I18" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L18" s="3">
+      <c r="L18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M18" s="3">
         <v>44243.506944444445</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P18" s="4"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="28"/>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>14</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D19" s="5">
         <v>2</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L19" s="3">
+      <c r="L19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M19" s="3">
         <v>44244.506944444445</v>
       </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P19" s="4"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="28"/>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>15</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D20" s="5">
         <v>2</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="I20" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L20" s="3">
+      <c r="L20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M20" s="3">
         <v>44245.506944444445</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P20" s="4"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="28"/>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>16</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D21" s="5">
         <v>2</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L21" s="3">
+      <c r="L21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M21" s="3">
         <v>44246.506944444445</v>
       </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P21" s="4"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="28"/>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>17</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D22" s="5">
         <v>2</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L22" s="3">
+      <c r="L22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M22" s="3">
         <v>44247.506944444445</v>
       </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P22" s="4"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="28"/>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>18</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23" s="5">
         <v>2</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="I23" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L23" s="3">
+      <c r="L23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M23" s="3">
         <v>44248.506944444445</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="P23" s="7"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+      <c r="T23" s="29"/>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>19</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D24" s="1">
         <v>1</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="I24" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J24" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L24" s="3">
+        <v>21</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M24" s="3">
         <v>44249.506944444445</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>20</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D25" s="1">
         <v>1</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="I25" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="J25" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L25" s="3">
+        <v>21</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M25" s="3">
         <v>44250.506944444445</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>21</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D26" s="1">
         <v>1</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="I26" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="J26" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L26" s="3">
+        <v>21</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M26" s="3">
         <v>44251.506944444445</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>22</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D27" s="1">
         <v>1</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="I27" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L27" s="3">
+        <v>21</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M27" s="3">
         <v>44252.506944444445</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>23</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D28" s="1">
         <v>3</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="I28" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J28" s="1" t="s">
+      <c r="K28" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K28" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L28" s="3">
+      <c r="L28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M28" s="3">
         <v>44253.506944444445</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>24</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D29" s="1">
         <v>3</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="I29" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J29" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K29" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L29" s="3">
+      <c r="L29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M29" s="3">
         <v>44254.506944444445</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>25</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D30" s="1">
         <v>3</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="I30" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="K30" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K30" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L30" s="3">
+      <c r="L30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M30" s="3">
         <v>44255.506944444445</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>26</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D31" s="1">
         <v>3</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="K31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K31" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L31" s="3">
+      <c r="L31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M31" s="3">
         <v>44256.506944444445</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B32" s="1">
         <v>27</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D32" s="1">
         <v>3</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="J32" s="1" t="s">
+      <c r="K32" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K32" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L32" s="3">
+      <c r="L32" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M32" s="3">
         <v>44257.506944444445</v>
       </c>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
         <v>28</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D33" s="1">
         <v>3</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="I33" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="J33" s="1" t="s">
+      <c r="K33" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K33" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L33" s="3">
+      <c r="L33" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M33" s="3">
         <v>44258.506944444445</v>
       </c>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
         <v>29</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D34" s="1">
         <v>3</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="I34" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="J34" s="1" t="s">
+      <c r="K34" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K34" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L34" s="3">
+      <c r="L34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M34" s="3">
         <v>44259.506944444445</v>
       </c>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
         <v>30</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D35" s="1">
         <v>3</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="I35" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="J35" s="1" t="s">
+      <c r="K35" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K35" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L35" s="3">
+      <c r="L35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M35" s="3">
         <v>44260.506944444445</v>
       </c>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
         <v>31</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D36" s="1">
         <v>3</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="I36" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="K36" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K36" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L36" s="3">
+      <c r="L36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M36" s="3">
         <v>44261.506944444445</v>
       </c>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
         <v>32</v>
       </c>
-      <c r="C37" s="1">
-        <v>5</v>
-      </c>
-      <c r="E37" s="2" t="s">
+      <c r="C37" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D37" s="1">
+        <v>5</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="I37" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="J37" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K37" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L37" s="17">
-        <v>44263.840277777781</v>
-      </c>
-      <c r="P37" s="18"/>
-    </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M37" s="17">
+        <v>44263.840277777781</v>
+      </c>
+      <c r="Q37" s="18"/>
+    </row>
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
         <v>33</v>
       </c>
-      <c r="C38" s="1">
-        <v>5</v>
-      </c>
-      <c r="E38" s="2" t="s">
+      <c r="C38" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D38" s="1">
+        <v>5</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="I38" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J38" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K38" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L38" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M38" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <v>34</v>
       </c>
-      <c r="C39" s="1">
-        <v>5</v>
-      </c>
-      <c r="E39" s="2" t="s">
+      <c r="C39" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D39" s="1">
+        <v>5</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="I39" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="J39" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K39" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L39" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M39" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B40" s="1">
         <v>35</v>
       </c>
-      <c r="C40" s="1">
-        <v>5</v>
-      </c>
-      <c r="E40" s="2" t="s">
+      <c r="C40" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D40" s="1">
+        <v>5</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="I40" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="J40" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K40" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L40" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M40" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
         <v>36</v>
       </c>
-      <c r="C41" s="1">
-        <v>5</v>
-      </c>
-      <c r="E41" s="2" t="s">
+      <c r="C41" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D41" s="1">
+        <v>5</v>
+      </c>
+      <c r="F41" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="I41" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="J41" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K41" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L41" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M41" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
         <v>37</v>
       </c>
-      <c r="C42" s="1">
-        <v>5</v>
-      </c>
-      <c r="E42" s="2" t="s">
+      <c r="C42" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D42" s="1">
+        <v>5</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="I42" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="J42" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K42" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L42" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M42" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B43" s="1">
         <v>38</v>
       </c>
-      <c r="C43" s="1">
-        <v>5</v>
-      </c>
-      <c r="E43" s="2" t="s">
+      <c r="C43" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D43" s="1">
+        <v>5</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="I43" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="J43" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K43" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L43" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M43" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B44" s="1">
         <v>39</v>
       </c>
-      <c r="C44" s="1">
-        <v>5</v>
-      </c>
-      <c r="E44" s="2" t="s">
+      <c r="C44" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D44" s="1">
+        <v>5</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="I44" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="J44" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K44" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L44" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M44" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B45" s="1">
         <v>40</v>
       </c>
-      <c r="C45" s="1">
-        <v>5</v>
-      </c>
-      <c r="E45" s="2" t="s">
+      <c r="C45" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D45" s="1">
+        <v>5</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="H45" s="2" t="s">
+      <c r="I45" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="J45" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K45" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L45" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M45" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B46" s="1">
         <v>41</v>
       </c>
-      <c r="C46" s="1">
-        <v>5</v>
-      </c>
-      <c r="E46" s="2" t="s">
+      <c r="C46" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D46" s="1">
+        <v>5</v>
+      </c>
+      <c r="F46" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="H46" s="2" t="s">
+      <c r="I46" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="J46" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K46" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L46" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M46" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B47" s="1">
         <v>42</v>
       </c>
-      <c r="C47" s="1">
-        <v>5</v>
-      </c>
-      <c r="E47" s="2" t="s">
+      <c r="C47" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D47" s="1">
+        <v>5</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="I47" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="J47" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K47" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L47" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M47" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B48" s="1">
         <v>43</v>
       </c>
-      <c r="C48" s="1">
-        <v>5</v>
-      </c>
-      <c r="E48" s="2" t="s">
+      <c r="C48" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D48" s="1">
+        <v>5</v>
+      </c>
+      <c r="F48" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="I48" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J48" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K48" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L48" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M48" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B49" s="1">
         <v>44</v>
       </c>
-      <c r="C49" s="1">
-        <v>5</v>
-      </c>
-      <c r="E49" s="2" t="s">
+      <c r="C49" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D49" s="1">
+        <v>5</v>
+      </c>
+      <c r="F49" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="I49" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="J49" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K49" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L49" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M49" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B50" s="1">
         <v>45</v>
       </c>
-      <c r="C50" s="1">
-        <v>5</v>
-      </c>
-      <c r="E50" s="2" t="s">
+      <c r="C50" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D50" s="1">
+        <v>5</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="H50" s="2" t="s">
+      <c r="I50" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="J50" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K50" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L50" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M50" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B51" s="1">
         <v>46</v>
       </c>
-      <c r="C51" s="1">
-        <v>5</v>
-      </c>
-      <c r="E51" s="2" t="s">
+      <c r="C51" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D51" s="1">
+        <v>5</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H51" s="2" t="s">
+      <c r="I51" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="J51" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K51" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L51" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M51" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B52" s="1">
         <v>47</v>
       </c>
-      <c r="C52" s="1">
-        <v>5</v>
-      </c>
-      <c r="E52" s="2" t="s">
+      <c r="C52" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D52" s="1">
+        <v>5</v>
+      </c>
+      <c r="F52" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="H52" s="2" t="s">
+      <c r="I52" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="J52" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K52" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L52" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M52" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B53" s="1">
         <v>48</v>
       </c>
-      <c r="C53" s="1">
-        <v>5</v>
-      </c>
-      <c r="E53" s="2" t="s">
+      <c r="C53" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D53" s="1">
+        <v>5</v>
+      </c>
+      <c r="F53" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="H53" s="2" t="s">
+      <c r="I53" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="J53" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K53" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L53" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M53" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B54" s="1">
         <v>49</v>
       </c>
-      <c r="C54" s="1">
-        <v>5</v>
-      </c>
-      <c r="E54" s="2" t="s">
+      <c r="C54" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D54" s="1">
+        <v>5</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="H54" s="2" t="s">
+      <c r="I54" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="J54" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K54" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L54" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M54" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B55" s="1">
         <v>50</v>
       </c>
-      <c r="C55" s="1">
-        <v>5</v>
-      </c>
-      <c r="E55" s="2" t="s">
+      <c r="C55" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D55" s="1">
+        <v>5</v>
+      </c>
+      <c r="F55" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="H55" s="2" t="s">
+      <c r="I55" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="J55" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K55" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L55" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M55" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B56" s="1">
         <v>51</v>
       </c>
-      <c r="C56" s="1">
-        <v>5</v>
-      </c>
-      <c r="E56" s="2" t="s">
+      <c r="C56" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D56" s="1">
+        <v>5</v>
+      </c>
+      <c r="F56" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="H56" s="2" t="s">
+      <c r="I56" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="J56" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K56" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L56" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M56" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B57" s="1">
         <v>52</v>
       </c>
-      <c r="C57" s="1">
-        <v>5</v>
-      </c>
-      <c r="E57" s="2" t="s">
+      <c r="C57" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D57" s="1">
+        <v>5</v>
+      </c>
+      <c r="F57" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="H57" s="2" t="s">
+      <c r="I57" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="J57" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K57" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L57" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M57" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B58" s="1">
         <v>53</v>
       </c>
-      <c r="C58" s="1">
-        <v>5</v>
-      </c>
-      <c r="E58" s="2" t="s">
+      <c r="C58" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D58" s="1">
+        <v>5</v>
+      </c>
+      <c r="F58" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="H58" s="2" t="s">
+      <c r="I58" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="J58" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K58" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L58" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M58" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B59" s="1">
         <v>54</v>
       </c>
-      <c r="C59" s="1">
-        <v>5</v>
-      </c>
-      <c r="E59" s="2" t="s">
+      <c r="C59" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D59" s="1">
+        <v>5</v>
+      </c>
+      <c r="F59" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="H59" s="2" t="s">
+      <c r="I59" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="J59" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K59" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L59" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M59" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B60" s="1">
         <v>55</v>
       </c>
-      <c r="C60" s="1">
-        <v>5</v>
-      </c>
-      <c r="E60" s="2" t="s">
+      <c r="C60" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D60" s="1">
+        <v>5</v>
+      </c>
+      <c r="F60" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="H60" s="2" t="s">
+      <c r="I60" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="J60" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K60" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L60" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M60" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="61" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B61" s="1">
         <v>56</v>
       </c>
-      <c r="C61" s="1">
-        <v>5</v>
-      </c>
-      <c r="E61" s="2" t="s">
+      <c r="C61" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D61" s="1">
+        <v>5</v>
+      </c>
+      <c r="F61" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="H61" s="2" t="s">
+      <c r="I61" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="J61" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K61" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L61" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M61" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="62" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B62" s="1">
         <v>57</v>
       </c>
-      <c r="C62" s="1">
-        <v>5</v>
-      </c>
-      <c r="E62" s="2" t="s">
+      <c r="C62" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D62" s="1">
+        <v>5</v>
+      </c>
+      <c r="F62" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="H62" s="2" t="s">
+      <c r="I62" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="J62" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K62" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L62" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M62" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B63" s="1">
         <v>58</v>
       </c>
-      <c r="C63" s="1">
-        <v>5</v>
-      </c>
-      <c r="E63" s="2" t="s">
+      <c r="C63" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D63" s="1">
+        <v>5</v>
+      </c>
+      <c r="F63" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="H63" s="2" t="s">
+      <c r="I63" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="J63" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K63" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L63" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L63" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M63" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B64" s="1">
         <v>59</v>
       </c>
-      <c r="C64" s="1">
-        <v>5</v>
-      </c>
-      <c r="E64" s="2" t="s">
+      <c r="C64" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D64" s="1">
+        <v>5</v>
+      </c>
+      <c r="F64" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="H64" s="2" t="s">
+      <c r="I64" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="J64" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K64" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L64" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M64" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="65" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B65" s="1">
         <v>60</v>
       </c>
-      <c r="C65" s="1">
-        <v>5</v>
-      </c>
-      <c r="E65" s="2" t="s">
+      <c r="C65" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D65" s="1">
+        <v>5</v>
+      </c>
+      <c r="F65" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H65" s="2" t="s">
+      <c r="I65" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="J65" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K65" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L65" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M65" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="66" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B66" s="1">
         <v>61</v>
       </c>
-      <c r="C66" s="1">
-        <v>5</v>
-      </c>
-      <c r="E66" s="2" t="s">
+      <c r="C66" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D66" s="1">
+        <v>5</v>
+      </c>
+      <c r="F66" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="H66" s="2" t="s">
+      <c r="I66" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="J66" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K66" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L66" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L66" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M66" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="67" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B67" s="1">
         <v>62</v>
       </c>
-      <c r="C67" s="1">
-        <v>5</v>
-      </c>
-      <c r="E67" s="2" t="s">
+      <c r="C67" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D67" s="1">
+        <v>5</v>
+      </c>
+      <c r="F67" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H67" s="2" t="s">
+      <c r="I67" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="J67" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K67" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L67" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L67" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M67" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="68" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B68" s="1">
         <v>63</v>
       </c>
-      <c r="C68" s="1">
-        <v>5</v>
-      </c>
-      <c r="E68" s="2" t="s">
+      <c r="C68" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D68" s="1">
+        <v>5</v>
+      </c>
+      <c r="F68" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="H68" s="2" t="s">
+      <c r="I68" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="J68" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K68" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L68" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L68" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M68" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="69" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B69" s="1">
         <v>64</v>
       </c>
-      <c r="C69" s="1">
-        <v>5</v>
-      </c>
-      <c r="E69" s="2" t="s">
+      <c r="C69" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D69" s="1">
+        <v>5</v>
+      </c>
+      <c r="F69" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="H69" s="2" t="s">
+      <c r="I69" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="J69" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K69" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L69" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L69" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M69" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="70" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B70" s="1">
         <v>65</v>
       </c>
-      <c r="C70" s="1">
-        <v>5</v>
-      </c>
-      <c r="E70" s="2" t="s">
+      <c r="C70" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D70" s="1">
+        <v>5</v>
+      </c>
+      <c r="F70" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="H70" s="2" t="s">
+      <c r="I70" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="J70" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K70" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L70" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L70" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M70" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="71" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B71" s="1">
         <v>66</v>
       </c>
-      <c r="C71" s="1">
-        <v>5</v>
-      </c>
-      <c r="E71" s="2" t="s">
+      <c r="C71" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D71" s="1">
+        <v>5</v>
+      </c>
+      <c r="F71" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="H71" s="2" t="s">
+      <c r="I71" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="J71" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K71" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L71" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L71" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M71" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="72" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B72" s="1">
         <v>67</v>
       </c>
-      <c r="C72" s="1">
-        <v>5</v>
-      </c>
-      <c r="E72" s="2" t="s">
+      <c r="C72" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D72" s="1">
+        <v>5</v>
+      </c>
+      <c r="F72" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="H72" s="2" t="s">
+      <c r="I72" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="J72" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K72" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L72" s="17">
-        <v>44263.840277777781</v>
-      </c>
-    </row>
-    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="L72" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M72" s="17">
+        <v>44263.840277777781</v>
+      </c>
+    </row>
+    <row r="73" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B73" s="1">
         <v>68</v>
       </c>
-      <c r="C73" s="1">
-        <v>5</v>
-      </c>
-      <c r="E73" s="2" t="s">
+      <c r="C73" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D73" s="1">
+        <v>5</v>
+      </c>
+      <c r="F73" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H73" s="2" t="s">
+      <c r="I73" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="J73" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K73" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L73" s="17">
+        <v>21</v>
+      </c>
+      <c r="L73" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M73" s="17">
         <v>44272.416666666664</v>
       </c>
     </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B74" s="1">
         <v>69</v>
       </c>
-      <c r="C74" s="1">
-        <v>5</v>
-      </c>
-      <c r="E74" s="2" t="s">
+      <c r="C74" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D74" s="1">
+        <v>5</v>
+      </c>
+      <c r="F74" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="H74" s="2" t="s">
+      <c r="I74" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="J74" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K74" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L74" s="17">
+        <v>21</v>
+      </c>
+      <c r="L74" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M74" s="17">
         <v>44272.416666666664</v>
       </c>
     </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B75" s="1">
         <v>70</v>
       </c>
-      <c r="C75" s="1">
-        <v>5</v>
-      </c>
-      <c r="E75" s="2" t="s">
+      <c r="C75" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D75" s="1">
+        <v>5</v>
+      </c>
+      <c r="F75" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="H75" s="2" t="s">
+      <c r="I75" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="J75" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K75" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L75" s="17">
+        <v>21</v>
+      </c>
+      <c r="L75" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M75" s="17">
         <v>44272.416666666664</v>
       </c>
     </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B76" s="1">
         <v>71</v>
       </c>
-      <c r="C76" s="1">
-        <v>5</v>
-      </c>
-      <c r="E76" s="2" t="s">
+      <c r="C76" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D76" s="1">
+        <v>5</v>
+      </c>
+      <c r="F76" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="H76" s="2" t="s">
+      <c r="I76" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="J76" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="K76" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L76" s="17">
+        <v>21</v>
+      </c>
+      <c r="L76" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M76" s="17">
         <v>44272.416666666664</v>
       </c>
     </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L77" s="17"/>
-    </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L78" s="17"/>
-    </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L79" s="17"/>
-    </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L80" s="17"/>
+    <row r="77" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M77" s="17"/>
+    </row>
+    <row r="78" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M78" s="17"/>
+    </row>
+    <row r="79" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M79" s="17"/>
+    </row>
+    <row r="80" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="M80" s="17"/>
     </row>
   </sheetData>
-  <autoFilter ref="B5:L76" xr:uid="{2F20A0F7-DAF3-43D5-A4BA-DE7B4D342869}"/>
+  <autoFilter ref="B5:M76" xr:uid="{2F20A0F7-DAF3-43D5-A4BA-DE7B4D342869}"/>
+  <hyperlinks>
+    <hyperlink ref="R15" r:id="rId1" xr:uid="{107D487D-9538-4712-A872-C2C03526F110}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
04.07. brain teaset update
</commit_message>
<xml_diff>
--- a/data-structur.xlsx
+++ b/data-structur.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\Projects\WebDev\2021\210206_BirDict\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530F9B66-BFE3-4165-8CA3-797A8E8E875C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56CB41F-6D7E-4F9C-9C2D-FE3632BF5560}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="1635" windowWidth="25740" windowHeight="18105" activeTab="1" xr2:uid="{784D83DC-DBDD-470F-9266-ADF61A2E4B6A}"/>
+    <workbookView xWindow="22275" yWindow="2895" windowWidth="25815" windowHeight="15480" xr2:uid="{784D83DC-DBDD-470F-9266-ADF61A2E4B6A}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -1229,8 +1229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB3B0B2-54B0-4330-B127-9A7406DC2F48}">
   <dimension ref="B5:S76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3060,8 +3060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{325C7FCC-0F46-4B23-9498-862573592E5F}">
   <dimension ref="C4:K83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="K66" sqref="K66"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3071,7 +3071,7 @@
     <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="31.7109375" customWidth="1"/>
     <col min="7" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" customWidth="1"/>
     <col min="11" max="11" width="63" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4879,7 +4879,7 @@
         <v>44263.840277777781</v>
       </c>
       <c r="K70" t="str">
-        <f t="shared" ref="K70:K83" si="1">"('"&amp;D70&amp;"',"&amp;"'"&amp;E70&amp;"',"&amp;"'"&amp;F70&amp;"',"&amp;""&amp;G70&amp;","&amp;H70&amp;",GETDATE()),"</f>
+        <f t="shared" ref="K70:K71" si="1">"('"&amp;D70&amp;"',"&amp;"'"&amp;E70&amp;"',"&amp;"'"&amp;F70&amp;"',"&amp;""&amp;G70&amp;","&amp;H70&amp;",GETDATE()),"</f>
         <v>('5','calf','vádli',3,1,GETDATE()),</v>
       </c>
     </row>

</xml_diff>